<commit_message>
Updated the gradient calculation after understanding the weird colour mapping of ue4
</commit_message>
<xml_diff>
--- a/docs/ue4_color_mapping.xlsx
+++ b/docs/ue4_color_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\LavalVirtual2020\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A3E21F3-D97B-4A16-A353-85256ADBA31E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6F07D-7C74-43E3-AD06-4890C7987370}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10605" yWindow="3585" windowWidth="21570" windowHeight="11385" xr2:uid="{2AC42075-0BAD-4696-8E6A-6A00EC7A8A6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AC42075-0BAD-4696-8E6A-6A00EC7A8A6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -204,7 +208,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$105</c:f>
+              <c:f>Sheet1!$A$5:$A$105</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="101"/>
@@ -516,7 +520,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$105</c:f>
+              <c:f>Sheet1!$B$5:$B$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -587,9 +591,59 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13483119703592145"/>
+                  <c:y val="2.6089317545951434E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$105</c:f>
+              <c:f>Sheet1!$A$5:$A$105</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="101"/>
@@ -901,39 +955,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$5:$I$105</c:f>
+              <c:f>Sheet1!$C$5:$C$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="1">
-                  <c:v>5.5677643628300215</c:v>
+                  <c:v>0.12156862745098039</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.6811457478686078</c:v>
+                  <c:v>0.23137254901960785</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.3808315196468595</c:v>
+                  <c:v>0.34509803921568627</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.045361017187261</c:v>
+                  <c:v>0.47843137254901963</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.180339887498949</c:v>
+                  <c:v>0.49019607843137253</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11.61895003862225</c:v>
+                  <c:v>0.52941176470588236</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>13.638181696985855</c:v>
+                  <c:v>0.72941176470588232</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>14.212670403551895</c:v>
+                  <c:v>0.792156862745098</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>14.966629547095765</c:v>
+                  <c:v>0.8784313725490196</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>15.968719422671311</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -942,6 +996,441 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-AC18-4471-8783-FFA1A1FE24B0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.6430064225339816E-2"/>
+                  <c:y val="0.12400650068666454"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$105</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="1">
+                  <c:v>9.9809695375745241E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0758109075041078E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.7682672140879973E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.19952591299168229</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21040926236891394</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.24896494862092322</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.50167385055101688</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.60086089203632775</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75323438068507542</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E616-4208-8604-26BE92BD3423}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1692,16 +2181,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>72</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2026,587 +2515,627 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6E5449-3382-4E57-9EFC-21F9677D51BA}">
-  <dimension ref="G5:I105"/>
+  <dimension ref="A5:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="I8" sqref="I7:I8"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G5" s="1">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G6" s="1">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>0.01</v>
       </c>
-      <c r="H6">
+      <c r="B6">
         <v>31</v>
       </c>
-      <c r="I6">
-        <f>SQRT(H6)</f>
-        <v>5.5677643628300215</v>
-      </c>
-    </row>
-    <row r="7" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="1">
+      <c r="C6">
+        <f>B6/255</f>
+        <v>0.12156862745098039</v>
+      </c>
+      <c r="D6">
+        <f>C6^2.18627</f>
+        <v>9.9809695375745241E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="1">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G9" s="1">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>0.04</v>
       </c>
-      <c r="H9">
+      <c r="B9">
         <v>59</v>
       </c>
-      <c r="I9">
-        <f t="shared" ref="I7:I70" si="0">SQRT(H9)</f>
-        <v>7.6811457478686078</v>
-      </c>
-    </row>
-    <row r="10" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G10" s="1">
+      <c r="C9">
+        <f>B9/255</f>
+        <v>0.23137254901960785</v>
+      </c>
+      <c r="D9">
+        <f>C9^2.18627</f>
+        <v>4.0758109075041078E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G11" s="1">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G12" s="1">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G13" s="1">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G14" s="1">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>0.09</v>
       </c>
     </row>
-    <row r="15" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G15" s="1">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>0.1</v>
       </c>
-      <c r="H15">
+      <c r="B15">
         <v>88</v>
       </c>
-      <c r="I15">
+      <c r="C15">
+        <f>B15/255</f>
+        <v>0.34509803921568627</v>
+      </c>
+      <c r="D15">
+        <f>C15^2.18627</f>
+        <v>9.7682672140879973E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B25">
+        <v>122</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C26" si="0">B25/255</f>
+        <v>0.47843137254901963</v>
+      </c>
+      <c r="D25">
+        <f>C25^2.18627</f>
+        <v>0.19952591299168229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="B26">
+        <v>125</v>
+      </c>
+      <c r="C26">
         <f t="shared" si="0"/>
-        <v>9.3808315196468595</v>
-      </c>
-    </row>
-    <row r="16" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G16" s="1">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G17" s="1">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="1">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="1">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G20" s="1">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G21" s="1">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="1">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="1">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="1">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="H25">
-        <v>122</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="0"/>
-        <v>11.045361017187261</v>
-      </c>
-    </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="H26">
-        <v>125</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>11.180339887498949</v>
-      </c>
-    </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G27" s="1">
+        <v>0.49019607843137253</v>
+      </c>
+      <c r="D26">
+        <f>C26^2.18627</f>
+        <v>0.21040926236891394</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>0.22</v>
       </c>
     </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G28" s="1">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>0.23</v>
       </c>
     </row>
-    <row r="29" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="1">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>0.24</v>
       </c>
     </row>
-    <row r="30" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G30" s="1">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>0.25</v>
       </c>
-      <c r="H30">
+      <c r="B30">
         <v>135</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>11.61895003862225</v>
-      </c>
-    </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G31" s="1">
+      <c r="C30">
+        <f>B30/255</f>
+        <v>0.52941176470588236</v>
+      </c>
+      <c r="D30">
+        <f>C30^2.18627</f>
+        <v>0.24896494862092322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>0.26</v>
       </c>
     </row>
-    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G32" s="1">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>0.27</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G36" s="1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>0.31</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>0.32</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>0.33</v>
       </c>
     </row>
-    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>0.34</v>
       </c>
     </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>0.35</v>
       </c>
     </row>
-    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>0.36</v>
       </c>
     </row>
-    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>0.37</v>
       </c>
     </row>
-    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>0.38</v>
       </c>
     </row>
-    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G44" s="1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>0.39</v>
       </c>
     </row>
-    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G45" s="1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>0.4</v>
       </c>
     </row>
-    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G46" s="1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>0.41</v>
       </c>
     </row>
-    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>0.42</v>
       </c>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>0.43</v>
       </c>
     </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G49" s="1">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>0.44</v>
       </c>
     </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G50" s="1">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>0.45</v>
       </c>
     </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G51" s="1">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>0.46</v>
       </c>
     </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G52" s="1">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>0.47</v>
       </c>
     </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G53" s="1">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>0.48</v>
       </c>
     </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G54" s="1">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>0.49</v>
       </c>
     </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G55" s="1">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>0.5</v>
       </c>
-      <c r="H55">
+      <c r="B55">
         <v>186</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="0"/>
-        <v>13.638181696985855</v>
-      </c>
-    </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="1">
+      <c r="C55">
+        <f>B55/255</f>
+        <v>0.72941176470588232</v>
+      </c>
+      <c r="D55">
+        <f>C55^2.18627</f>
+        <v>0.50167385055101688</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>0.51</v>
       </c>
     </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G57" s="1">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>0.52</v>
       </c>
     </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G58" s="1">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>0.53</v>
       </c>
     </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G59" s="1">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G60" s="1">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G61" s="1">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G62" s="1">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G63" s="1">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G64" s="1">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>0.59</v>
       </c>
     </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G65" s="1">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>0.6</v>
       </c>
-      <c r="H65">
+      <c r="B65">
         <v>202</v>
       </c>
-      <c r="I65">
-        <f t="shared" si="0"/>
-        <v>14.212670403551895</v>
-      </c>
-    </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G66" s="1">
+      <c r="C65">
+        <f>B65/255</f>
+        <v>0.792156862745098</v>
+      </c>
+      <c r="D65">
+        <f>C65^2.18627</f>
+        <v>0.60086089203632775</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
         <v>0.61</v>
       </c>
     </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G67" s="1">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>0.62</v>
       </c>
     </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G68" s="1">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>0.63</v>
       </c>
     </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G69" s="1">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>0.64</v>
       </c>
     </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G70" s="1">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>0.65</v>
       </c>
     </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G71" s="1">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
         <v>0.66</v>
       </c>
     </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G72" s="1">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>0.67</v>
       </c>
     </row>
-    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G73" s="1">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
         <v>0.68</v>
       </c>
     </row>
-    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G74" s="1">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>0.69</v>
       </c>
     </row>
-    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G75" s="1">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>0.7</v>
       </c>
     </row>
-    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G76" s="1">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
         <v>0.71</v>
       </c>
     </row>
-    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G77" s="1">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>0.72</v>
       </c>
     </row>
-    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G78" s="1">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
         <v>0.73</v>
       </c>
     </row>
-    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G79" s="1">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>0.74</v>
       </c>
     </row>
-    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G80" s="1">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
         <v>0.75</v>
       </c>
-      <c r="H80">
+      <c r="B80">
         <v>224</v>
       </c>
-      <c r="I80">
-        <f t="shared" ref="I71:I105" si="1">SQRT(H80)</f>
-        <v>14.966629547095765</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G81" s="1">
+      <c r="C80">
+        <f>B80/255</f>
+        <v>0.8784313725490196</v>
+      </c>
+      <c r="D80">
+        <f>C80^2.18627</f>
+        <v>0.75323438068507542</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
         <v>0.76</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G82" s="1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
         <v>0.77</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G83" s="1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>0.78</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G84" s="1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>0.79</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G85" s="1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
         <v>0.8</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G86" s="1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>0.81</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G87" s="1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>0.82</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G88" s="1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <v>0.83</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G89" s="1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>0.84</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G90" s="1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
         <v>0.85</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G91" s="1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>0.86</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G92" s="1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>0.87</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G93" s="1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>0.88</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G94" s="1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
         <v>0.89</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G95" s="1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
         <v>0.9</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G96" s="1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
         <v>0.91</v>
       </c>
     </row>
-    <row r="97" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G97" s="1">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
         <v>0.92</v>
       </c>
     </row>
-    <row r="98" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G98" s="1">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
         <v>0.93</v>
       </c>
     </row>
-    <row r="99" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G99" s="1">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
         <v>0.94</v>
       </c>
     </row>
-    <row r="100" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G100" s="1">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
         <v>0.95</v>
       </c>
     </row>
-    <row r="101" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G101" s="1">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
         <v>0.96</v>
       </c>
     </row>
-    <row r="102" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G102" s="1">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
         <v>0.97</v>
       </c>
     </row>
-    <row r="103" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G103" s="1">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
         <v>0.98</v>
       </c>
     </row>
-    <row r="104" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G104" s="1">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
         <v>0.99</v>
       </c>
     </row>
-    <row r="105" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G105" s="1">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
         <v>1</v>
       </c>
-      <c r="H105">
+      <c r="B105">
         <v>255</v>
       </c>
-      <c r="I105">
-        <f t="shared" si="1"/>
-        <v>15.968719422671311</v>
+      <c r="C105">
+        <f>B105/255</f>
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <f>C105^2.18627</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2616,6 +3145,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F56A6FE9DCC9944EBB07588504B8BA9D" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c349da9de5c6b531770ad3cb81153917">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ef13d3fc-ffc2-4cc3-b65c-0757b7661eb4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f78de9fd77adce0ac7c4e105fdffe0f5" ns3:_="">
     <xsd:import namespace="ef13d3fc-ffc2-4cc3-b65c-0757b7661eb4"/>
@@ -2747,22 +3291,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D83EB60-E7A5-4B51-9BFA-C2C83F18813F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="ef13d3fc-ffc2-4cc3-b65c-0757b7661eb4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{875E3241-047B-4E20-B398-9F8231D685FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{306493A6-590F-422A-82F2-A26BFFCF4F52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2778,28 +3331,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{875E3241-047B-4E20-B398-9F8231D685FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D83EB60-E7A5-4B51-9BFA-C2C83F18813F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ef13d3fc-ffc2-4cc3-b65c-0757b7661eb4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Started working the the racquet design
</commit_message>
<xml_diff>
--- a/docs/ue4_color_mapping.xlsx
+++ b/docs/ue4_color_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\LavalVirtual2020\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6F07D-7C74-43E3-AD06-4890C7987370}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D0D965-8482-43AA-93B9-FC5FF379D0B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2AC42075-0BAD-4696-8E6A-6A00EC7A8A6E}"/>
   </bookViews>
@@ -28,10 +28,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,31 +521,301 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>31.027028201467857</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.602128741116701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.283238450245264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59</c:v>
+                  <c:v>58.495495008085214</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.781210716582734</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.415223544205745</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75.559317064005128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80.318121120987684</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.763855850696459</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88</c:v>
+                  <c:v>88.948817818868761</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92.912296504569468</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>96.68468405307496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100.29005506827761</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>103.74785919714078</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>107.07407279556756</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>110.28200683683409</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>113.38288859214268</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>116.38628991783337</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>119.30044881392611</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>122</c:v>
+                  <c:v>122.13251502798806</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>125</c:v>
+                  <c:v>124.88874051907246</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>127.57462917873698</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>130.19505596747672</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>132.75436276325132</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>135</c:v>
+                  <c:v>135.25643624830809</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>137.70477177928103</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140.10252620158559</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>142.45256185775281</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>144.75748351804961</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>147.0196695749504</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>149.24129855274251</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>151.42437176336631</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>153.57073277092996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>155.68208419695307</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>157.76000229673409</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>159.80594965733451</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>161.82128630440332</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>163.80727945460919</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>165.76511210994394</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>167.69589065744188</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>169.60065161127321</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>171.4803676124462</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>173.33595278350583</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>175.16826752088539</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>176.97812279534509</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>178.76628402074732</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>180.53347454289678</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>182.28037879300933</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>184.00764514433132</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>186</c:v>
+                  <c:v>185.71588850531492</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>187.40569267840368</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>189.0776125097758</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>190.73217585221715</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>192.36988536057268</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>193.99122013687983</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>195.59663724026169</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>197.18657307490417</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>198.76144466791945</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>200.32165084757125</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>202</c:v>
+                  <c:v>201.8675733311824</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>203.39957773103157</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>204.91801448566</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>206.42321972322836</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>207.91551606287771</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>209.39521335944178</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>210.86260939632214</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>212.31799053086218</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>213.76163229613445</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>215.19379996268108</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>216.61474906341093</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>218.02472588456112</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>219.42396792536186</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>220.81270432880524</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>222.19115628570421</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>224</c:v>
+                  <c:v>223.55953741403536</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>224.91805411538559</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>226.26690591016688</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>227.60628575312228</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>228.93638033051877</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>230.25737034030814</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>231.5694307564313</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>232.87273107834804</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>234.16743556678793</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>235.45370346663884</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>236.73168921781988</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>238.00154265491952</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>239.26340919632082</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>240.51743002348155</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>241.76374225098729</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>243.0024790879508</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>244.2337699912886</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>245.4577408113683</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>246.6745139304852</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>247.88420839459405</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>249.0869400386924</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>250.28282160622538</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>251.47196286285589</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>252.65447070492115</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>253.83044926287562</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>255</c:v>
@@ -960,31 +1226,301 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="1">
-                  <c:v>0.12156862745098039</c:v>
+                  <c:v>0.12167462039791317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16706717153379097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20111073902056967</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23137254901960785</c:v>
+                  <c:v>0.2293940980709224</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25404396359444209</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27613813154590489</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29631104730982405</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31497302400387328</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33240727784586849</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.34509803921568627</c:v>
+                  <c:v>0.34881889340732847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36436194707674302</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.37915562373754885</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39329433360108867</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.40685434979270896</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41989832468850025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.43247845818366309</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.4446387787927164</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.45641682320718968</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.46784489730951417</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.47843137254901963</c:v>
+                  <c:v>0.47895103932544336</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.49019607843137253</c:v>
+                  <c:v>0.4897597667414606</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.50029266344602741</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.51056884693128124</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.52060534416961302</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.52941176470588236</c:v>
+                  <c:v>0.5304173970521886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.54001871285992564</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.54942167137876707</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.55863749748138358</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.56767640595313573</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.57654772382333486</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.58525999432448039</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.59382106573869142</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.60223816772913707</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.6105179772429532</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.618666675673467</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.62668999865621378</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.63459327962511103</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.64238148805729089</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.65005926317625073</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.65763094375467401</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.6651005945540126</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.67247202985273025</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.67974883444512091</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.68693438243484473</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.6940318540993925</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.70104425106175416</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.70797440997214423</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.71482501487454642</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.72159860840914247</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.72941176470588232</c:v>
+                  <c:v>0.72829760198162719</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.73492428501334772</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.74148083337166981</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.74796931706751824</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.7543917072963634</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.76074988288972478</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.76704563623632038</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.77328067872511441</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.77945664575654683</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.78557510136302455</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.792156862745098</c:v>
+                  <c:v>0.79163754247522511</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.79764540286679042</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.80360005680650981</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.80950282244403282</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.81535496495246162</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.82115769944879136</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.82691219371106728</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.8326195707092634</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.83828091096523316</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.84389725475561206</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.84946960417023898</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.85499892503749464</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.86048614872690932</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.86593217383845189</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.87133786778707534</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.8784313725490196</c:v>
+                  <c:v>0.87670406829033476</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.88203158476621801</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.88732119964771328</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.89257366962008733</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.89778972678634816</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.90297007976591426</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.90811541473110313</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.9132263963856786</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.91830366888936443</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.92334785673191699</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.92835956556007793</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.9333393829604687</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.93828787920125811</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.94320560793522179</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.94809310686661685</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.95295089838412084</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.9577794901619161</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.96257937573085606</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.96735103502151065</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.97209493488076104</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.97681152956349959</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.98150126120088388</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.98616456024649368</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.99080184590165155</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.99541352652108084</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>1</c:v>
@@ -1394,36 +1930,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
-                <c:pt idx="1">
-                  <c:v>9.9809695375745241E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.0758109075041078E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.7682672140879973E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.19952591299168229</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.21040926236891394</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.24896494862092322</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.50167385055101688</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.60086089203632775</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.75323438068507542</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2515,614 +3021,1307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6E5449-3382-4E57-9EFC-21F9677D51BA}">
-  <dimension ref="A5:D105"/>
+  <dimension ref="A5:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.01</v>
       </c>
       <c r="B6">
-        <v>31</v>
+        <f t="shared" ref="B6:B69" si="0">255*A6^0.4574</f>
+        <v>31.027028201467857</v>
       </c>
       <c r="C6">
         <f>B6/255</f>
-        <v>0.12156862745098039</v>
-      </c>
-      <c r="D6">
-        <f>C6^2.18627</f>
-        <v>9.9809695375745241E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.12167462039791317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>42.602128741116701</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C70" si="1">B7/255</f>
+        <v>0.16706717153379097</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>51.283238450245264</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.20111073902056967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.04</v>
       </c>
       <c r="B9">
-        <v>59</v>
+        <f t="shared" si="0"/>
+        <v>58.495495008085214</v>
       </c>
       <c r="C9">
-        <f>B9/255</f>
-        <v>0.23137254901960785</v>
-      </c>
-      <c r="D9">
-        <f>C9^2.18627</f>
-        <v>4.0758109075041078E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.2293940980709224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>64.781210716582734</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.25404396359444209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>70.415223544205745</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.27613813154590489</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>75.559317064005128</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.29631104730982405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>80.318121120987684</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.31497302400387328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>84.763855850696459</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.33240727784586849</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.1</v>
       </c>
       <c r="B15">
-        <v>88</v>
+        <f t="shared" si="0"/>
+        <v>88.948817818868761</v>
       </c>
       <c r="C15">
-        <f>B15/255</f>
-        <v>0.34509803921568627</v>
-      </c>
-      <c r="D15">
-        <f>C15^2.18627</f>
-        <v>9.7682672140879973E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.34881889340732847</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>92.912296504569468</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.36436194707674302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>96.68468405307496</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.37915562373754885</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>100.29005506827761</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.39329433360108867</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>103.74785919714078</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.40685434979270896</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>107.07407279556756</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0.41989832468850025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>110.28200683683409</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0.43247845818366309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>113.38288859214268</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0.4446387787927164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>116.38628991783337</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.45641682320718968</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>119.30044881392611</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.46784489730951417</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0.2</v>
       </c>
       <c r="B25">
-        <v>122</v>
+        <f t="shared" si="0"/>
+        <v>122.13251502798806</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C26" si="0">B25/255</f>
-        <v>0.47843137254901963</v>
-      </c>
-      <c r="D25">
-        <f>C25^2.18627</f>
-        <v>0.19952591299168229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.47895103932544336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0.21</v>
       </c>
       <c r="B26">
-        <v>125</v>
+        <f t="shared" si="0"/>
+        <v>124.88874051907246</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>0.49019607843137253</v>
-      </c>
-      <c r="D26">
-        <f>C26^2.18627</f>
-        <v>0.21040926236891394</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.4897597667414606</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>127.57462917873698</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0.50029266344602741</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>130.19505596747672</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0.51056884693128124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>132.75436276325132</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>0.52060534416961302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>0.25</v>
       </c>
       <c r="B30">
-        <v>135</v>
+        <f t="shared" si="0"/>
+        <v>135.25643624830809</v>
       </c>
       <c r="C30">
-        <f>B30/255</f>
-        <v>0.52941176470588236</v>
-      </c>
-      <c r="D30">
-        <f>C30^2.18627</f>
-        <v>0.24896494862092322</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.5304173970521886</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>137.70477177928103</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>0.54001871285992564</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>140.10252620158559</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>0.54942167137876707</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>142.45256185775281</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0.55863749748138358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>144.75748351804961</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>0.56767640595313573</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>147.0196695749504</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0.57654772382333486</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>149.24129855274251</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0.58525999432448039</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>151.42437176336631</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>0.59382106573869142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>153.57073277092996</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0.60223816772913707</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>155.68208419695307</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>0.6105179772429532</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>157.76000229673409</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>0.618666675673467</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>159.80594965733451</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>0.62668999865621378</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>161.82128630440332</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>0.63459327962511103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>163.80727945460919</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>0.64238148805729089</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>165.76511210994394</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>0.65005926317625073</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>167.69589065744188</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>0.65763094375467401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>169.60065161127321</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>0.6651005945540126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>171.4803676124462</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>0.67247202985273025</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>173.33595278350583</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>0.67974883444512091</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>175.16826752088539</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>0.68693438243484473</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>176.97812279534509</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>0.6940318540993925</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>178.76628402074732</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>0.70104425106175416</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>180.53347454289678</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>0.70797440997214423</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>182.28037879300933</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>0.71482501487454642</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>184.00764514433132</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>0.72159860840914247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>0.5</v>
       </c>
       <c r="B55">
-        <v>186</v>
+        <f t="shared" si="0"/>
+        <v>185.71588850531492</v>
       </c>
       <c r="C55">
-        <f>B55/255</f>
-        <v>0.72941176470588232</v>
-      </c>
-      <c r="D55">
-        <f>C55^2.18627</f>
-        <v>0.50167385055101688</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.72829760198162719</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>187.40569267840368</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>0.73492428501334772</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>189.0776125097758</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>0.74148083337166981</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>190.73217585221715</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>0.74796931706751824</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>192.36988536057268</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>0.7543917072963634</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>193.99122013687983</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>0.76074988288972478</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>195.59663724026169</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>0.76704563623632038</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>197.18657307490417</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>0.77328067872511441</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>198.76144466791945</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>0.77945664575654683</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>200.32165084757125</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>0.78557510136302455</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>0.6</v>
       </c>
       <c r="B65">
-        <v>202</v>
+        <f t="shared" si="0"/>
+        <v>201.8675733311824</v>
       </c>
       <c r="C65">
-        <f>B65/255</f>
-        <v>0.792156862745098</v>
-      </c>
-      <c r="D65">
-        <f>C65^2.18627</f>
-        <v>0.60086089203632775</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.79163754247522511</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>0.61</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>203.39957773103157</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>0.79764540286679042</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>204.91801448566</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="1"/>
+        <v>0.80360005680650981</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <f t="shared" si="0"/>
+        <v>206.42321972322836</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>0.80950282244403282</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <f t="shared" si="0"/>
+        <v>207.91551606287771</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>0.81535496495246162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <f t="shared" ref="B70:B80" si="2">255*A70^0.4574</f>
+        <v>209.39521335944178</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>0.82115769944879136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <f t="shared" si="2"/>
+        <v>210.86260939632214</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ref="C71:C104" si="3">B71/255</f>
+        <v>0.82691219371106728</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <f t="shared" si="2"/>
+        <v>212.31799053086218</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="3"/>
+        <v>0.8326195707092634</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <f t="shared" si="2"/>
+        <v>213.76163229613445</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="3"/>
+        <v>0.83828091096523316</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <f t="shared" si="2"/>
+        <v>215.19379996268108</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="3"/>
+        <v>0.84389725475561206</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <f t="shared" si="2"/>
+        <v>216.61474906341093</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="3"/>
+        <v>0.84946960417023898</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <f t="shared" si="2"/>
+        <v>218.02472588456112</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="3"/>
+        <v>0.85499892503749464</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <f t="shared" si="2"/>
+        <v>219.42396792536186</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="3"/>
+        <v>0.86048614872690932</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <f t="shared" si="2"/>
+        <v>220.81270432880524</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="3"/>
+        <v>0.86593217383845189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <f t="shared" si="2"/>
+        <v>222.19115628570421</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="3"/>
+        <v>0.87133786778707534</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>0.75</v>
       </c>
       <c r="B80">
-        <v>224</v>
+        <f t="shared" si="2"/>
+        <v>223.55953741403536</v>
       </c>
       <c r="C80">
-        <f>B80/255</f>
-        <v>0.8784313725490196</v>
-      </c>
-      <c r="D80">
-        <f>C80^2.18627</f>
-        <v>0.75323438068507542</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.87670406829033476</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <f t="shared" ref="B81:B89" si="4">255*A81^0.4574</f>
+        <v>224.91805411538559</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="3"/>
+        <v>0.88203158476621801</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <f t="shared" si="4"/>
+        <v>226.26690591016688</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="3"/>
+        <v>0.88732119964771328</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <f t="shared" si="4"/>
+        <v>227.60628575312228</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="3"/>
+        <v>0.89257366962008733</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <f t="shared" si="4"/>
+        <v>228.93638033051877</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="3"/>
+        <v>0.89778972678634816</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <f t="shared" si="4"/>
+        <v>230.25737034030814</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="3"/>
+        <v>0.90297007976591426</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <f t="shared" si="4"/>
+        <v>231.5694307564313</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="3"/>
+        <v>0.90811541473110313</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <f t="shared" si="4"/>
+        <v>232.87273107834804</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="3"/>
+        <v>0.9132263963856786</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>0.83</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <f t="shared" si="4"/>
+        <v>234.16743556678793</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="3"/>
+        <v>0.91830366888936443</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <f t="shared" si="4"/>
+        <v>235.45370346663884</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="3"/>
+        <v>0.92334785673191699</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <f>255*A90^0.4574</f>
+        <v>236.73168921781988</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="3"/>
+        <v>0.92835956556007793</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <f t="shared" ref="B91:B104" si="5">255*A91^0.4574</f>
+        <v>238.00154265491952</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="3"/>
+        <v>0.9333393829604687</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <f t="shared" si="5"/>
+        <v>239.26340919632082</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="3"/>
+        <v>0.93828787920125811</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <f t="shared" si="5"/>
+        <v>240.51743002348155</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="3"/>
+        <v>0.94320560793522179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <f t="shared" si="5"/>
+        <v>241.76374225098729</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="3"/>
+        <v>0.94809310686661685</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <f t="shared" si="5"/>
+        <v>243.0024790879508</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="3"/>
+        <v>0.95295089838412084</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>0.91</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <f t="shared" si="5"/>
+        <v>244.2337699912886</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="3"/>
+        <v>0.9577794901619161</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <f t="shared" si="5"/>
+        <v>245.4577408113683</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="3"/>
+        <v>0.96257937573085606</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <f t="shared" si="5"/>
+        <v>246.6745139304852</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="3"/>
+        <v>0.96735103502151065</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <f t="shared" si="5"/>
+        <v>247.88420839459405</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="3"/>
+        <v>0.97209493488076104</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <f t="shared" si="5"/>
+        <v>249.0869400386924</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="3"/>
+        <v>0.97681152956349959</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <f t="shared" si="5"/>
+        <v>250.28282160622538</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="3"/>
+        <v>0.98150126120088388</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <f t="shared" si="5"/>
+        <v>251.47196286285589</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="3"/>
+        <v>0.98616456024649368</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <f t="shared" si="5"/>
+        <v>252.65447070492115</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="3"/>
+        <v>0.99080184590165155</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <f t="shared" si="5"/>
+        <v>253.83044926287562</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="3"/>
+        <v>0.99541352652108084</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>1</v>
       </c>
@@ -3131,10 +4330,6 @@
       </c>
       <c r="C105">
         <f>B105/255</f>
-        <v>1</v>
-      </c>
-      <c r="D105">
-        <f>C105^2.18627</f>
         <v>1</v>
       </c>
     </row>
@@ -3151,15 +4346,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F56A6FE9DCC9944EBB07588504B8BA9D" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c349da9de5c6b531770ad3cb81153917">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ef13d3fc-ffc2-4cc3-b65c-0757b7661eb4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f78de9fd77adce0ac7c4e105fdffe0f5" ns3:_="">
     <xsd:import namespace="ef13d3fc-ffc2-4cc3-b65c-0757b7661eb4"/>
@@ -3291,6 +4477,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D83EB60-E7A5-4B51-9BFA-C2C83F18813F}">
   <ds:schemaRefs>
@@ -3308,14 +4503,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{875E3241-047B-4E20-B398-9F8231D685FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{306493A6-590F-422A-82F2-A26BFFCF4F52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3331,4 +4518,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{875E3241-047B-4E20-B398-9F8231D685FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>